<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI5-Sandbox@53c2227e69516abad84bd13993063f65bd643527 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-medicationdispense.xlsx
+++ b/StructureDefinition-us-core-medicationdispense.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2499" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2497" uniqueCount="503">
   <si>
     <t>Property</t>
   </si>
@@ -1229,9 +1229,6 @@
     <t>A code specifying the route or physiological path of administration of a therapeutic agent into or onto a patient's body.</t>
   </si>
   <si>
-    <t>A coded concept describing the route or physiological path of administration of a therapeutic agent into or onto the body of a subject.</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/ValueSet/route-codes</t>
   </si>
   <si>
@@ -1326,8 +1323,8 @@
     <t>MedicationDispense.dosageInstruction.doseAndRate.dose[x]</t>
   </si>
   <si>
-    <t>Range
-Quantity {SimpleQuantity}</t>
+    <t>Quantity {SimpleQuantity}
+Range</t>
   </si>
   <si>
     <t>Amount of medication per dose</t>
@@ -7320,7 +7317,7 @@
         <v>86</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="I47" t="s" s="2">
         <v>76</v>
@@ -7364,31 +7361,29 @@
         <v>76</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>174</v>
-      </c>
-      <c r="Y47" t="s" s="2">
+        <v>192</v>
+      </c>
+      <c r="Y47" s="2"/>
+      <c r="Z47" t="s" s="2">
         <v>389</v>
       </c>
-      <c r="Z47" t="s" s="2">
+      <c r="AA47" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB47" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC47" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD47" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE47" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AF47" t="s" s="2">
         <v>390</v>
-      </c>
-      <c r="AA47" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB47" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC47" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD47" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE47" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF47" t="s" s="2">
-        <v>391</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>77</v>
@@ -7406,24 +7401,24 @@
         <v>76</v>
       </c>
       <c r="AL47" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="AM47" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AN47" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AO47" t="s" s="2">
         <v>392</v>
-      </c>
-      <c r="AM47" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN47" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AO47" t="s" s="2">
-        <v>393</v>
       </c>
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7449,16 +7444,16 @@
         <v>180</v>
       </c>
       <c r="L48" t="s" s="2">
+        <v>394</v>
+      </c>
+      <c r="M48" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="M48" t="s" s="2">
+      <c r="N48" t="s" s="2">
         <v>396</v>
       </c>
-      <c r="N48" t="s" s="2">
+      <c r="O48" t="s" s="2">
         <v>397</v>
-      </c>
-      <c r="O48" t="s" s="2">
-        <v>398</v>
       </c>
       <c r="P48" t="s" s="2">
         <v>76</v>
@@ -7486,28 +7481,28 @@
         <v>174</v>
       </c>
       <c r="Y48" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="Z48" t="s" s="2">
         <v>399</v>
       </c>
-      <c r="Z48" t="s" s="2">
+      <c r="AA48" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB48" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC48" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD48" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE48" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AF48" t="s" s="2">
         <v>400</v>
-      </c>
-      <c r="AA48" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB48" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC48" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD48" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE48" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF48" t="s" s="2">
-        <v>401</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>77</v>
@@ -7525,24 +7520,24 @@
         <v>76</v>
       </c>
       <c r="AL48" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="AM48" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AN48" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AO48" t="s" s="2">
         <v>402</v>
-      </c>
-      <c r="AM48" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN48" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AO48" t="s" s="2">
-        <v>403</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7556,7 +7551,7 @@
         <v>78</v>
       </c>
       <c r="H49" t="s" s="2">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="I49" t="s" s="2">
         <v>76</v>
@@ -7565,13 +7560,13 @@
         <v>87</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>405</v>
       </c>
-      <c r="L49" t="s" s="2">
+      <c r="M49" t="s" s="2">
         <v>406</v>
-      </c>
-      <c r="M49" t="s" s="2">
-        <v>407</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -7622,7 +7617,7 @@
         <v>76</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>77</v>
@@ -7649,15 +7644,15 @@
         <v>76</v>
       </c>
       <c r="AO49" t="s" s="2">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7769,10 +7764,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7886,10 +7881,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7915,14 +7910,14 @@
         <v>180</v>
       </c>
       <c r="L52" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="M52" t="s" s="2">
         <v>413</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>414</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="P52" t="s" s="2">
         <v>76</v>
@@ -7950,28 +7945,28 @@
         <v>174</v>
       </c>
       <c r="Y52" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="Z52" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="Z52" t="s" s="2">
+      <c r="AA52" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AC52" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AD52" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AE52" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AF52" t="s" s="2">
         <v>417</v>
-      </c>
-      <c r="AA52" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AB52" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AC52" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AD52" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AE52" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF52" t="s" s="2">
-        <v>418</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>77</v>
@@ -7998,15 +7993,15 @@
         <v>76</v>
       </c>
       <c r="AO52" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -8020,7 +8015,7 @@
         <v>86</v>
       </c>
       <c r="H53" t="s" s="2">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="I53" t="s" s="2">
         <v>76</v>
@@ -8029,19 +8024,19 @@
         <v>87</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="L53" t="s" s="2">
         <v>421</v>
       </c>
-      <c r="L53" t="s" s="2">
+      <c r="M53" t="s" s="2">
         <v>422</v>
       </c>
-      <c r="M53" t="s" s="2">
+      <c r="N53" t="s" s="2">
         <v>423</v>
       </c>
-      <c r="N53" t="s" s="2">
+      <c r="O53" t="s" s="2">
         <v>424</v>
-      </c>
-      <c r="O53" t="s" s="2">
-        <v>425</v>
       </c>
       <c r="P53" t="s" s="2">
         <v>76</v>
@@ -8066,13 +8061,11 @@
         <v>76</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="Y53" t="s" s="2">
-        <v>76</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="Y53" s="2"/>
       <c r="Z53" t="s" s="2">
-        <v>76</v>
+        <v>278</v>
       </c>
       <c r="AA53" t="s" s="2">
         <v>76</v>
@@ -8090,7 +8083,7 @@
         <v>76</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>77</v>
@@ -8108,7 +8101,7 @@
         <v>76</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AM53" t="s" s="2">
         <v>76</v>
@@ -8117,15 +8110,15 @@
         <v>76</v>
       </c>
       <c r="AO53" t="s" s="2">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8148,19 +8141,19 @@
         <v>87</v>
       </c>
       <c r="K54" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="L54" t="s" s="2">
         <v>429</v>
       </c>
-      <c r="L54" t="s" s="2">
+      <c r="M54" t="s" s="2">
         <v>430</v>
       </c>
-      <c r="M54" t="s" s="2">
+      <c r="N54" t="s" s="2">
         <v>431</v>
       </c>
-      <c r="N54" t="s" s="2">
+      <c r="O54" t="s" s="2">
         <v>432</v>
-      </c>
-      <c r="O54" t="s" s="2">
-        <v>433</v>
       </c>
       <c r="P54" t="s" s="2">
         <v>76</v>
@@ -8209,7 +8202,7 @@
         <v>76</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>77</v>
@@ -8227,24 +8220,24 @@
         <v>76</v>
       </c>
       <c r="AL54" t="s" s="2">
+        <v>434</v>
+      </c>
+      <c r="AM54" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AN54" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AO54" t="s" s="2">
         <v>435</v>
-      </c>
-      <c r="AM54" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN54" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AO54" t="s" s="2">
-        <v>436</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8267,19 +8260,19 @@
         <v>87</v>
       </c>
       <c r="K55" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="L55" t="s" s="2">
         <v>438</v>
       </c>
-      <c r="L55" t="s" s="2">
+      <c r="M55" t="s" s="2">
         <v>439</v>
       </c>
-      <c r="M55" t="s" s="2">
+      <c r="N55" t="s" s="2">
         <v>440</v>
       </c>
-      <c r="N55" t="s" s="2">
+      <c r="O55" t="s" s="2">
         <v>441</v>
-      </c>
-      <c r="O55" t="s" s="2">
-        <v>442</v>
       </c>
       <c r="P55" t="s" s="2">
         <v>76</v>
@@ -8328,7 +8321,7 @@
         <v>76</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>77</v>
@@ -8346,24 +8339,24 @@
         <v>76</v>
       </c>
       <c r="AL55" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="AM55" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AN55" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AO55" t="s" s="2">
         <v>444</v>
-      </c>
-      <c r="AM55" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN55" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AO55" t="s" s="2">
-        <v>445</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8389,16 +8382,16 @@
         <v>275</v>
       </c>
       <c r="L56" t="s" s="2">
+        <v>446</v>
+      </c>
+      <c r="M56" t="s" s="2">
         <v>447</v>
       </c>
-      <c r="M56" t="s" s="2">
+      <c r="N56" t="s" s="2">
         <v>448</v>
       </c>
-      <c r="N56" t="s" s="2">
+      <c r="O56" t="s" s="2">
         <v>449</v>
-      </c>
-      <c r="O56" t="s" s="2">
-        <v>450</v>
       </c>
       <c r="P56" t="s" s="2">
         <v>76</v>
@@ -8447,7 +8440,7 @@
         <v>76</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>77</v>
@@ -8465,7 +8458,7 @@
         <v>76</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="AM56" t="s" s="2">
         <v>76</v>
@@ -8479,10 +8472,10 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8508,14 +8501,14 @@
         <v>275</v>
       </c>
       <c r="L57" t="s" s="2">
+        <v>453</v>
+      </c>
+      <c r="M57" t="s" s="2">
         <v>454</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>455</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="P57" t="s" s="2">
         <v>76</v>
@@ -8564,7 +8557,7 @@
         <v>76</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>77</v>
@@ -8582,7 +8575,7 @@
         <v>76</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="AM57" t="s" s="2">
         <v>76</v>
@@ -8596,10 +8589,10 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8625,10 +8618,10 @@
         <v>221</v>
       </c>
       <c r="L58" t="s" s="2">
+        <v>458</v>
+      </c>
+      <c r="M58" t="s" s="2">
         <v>459</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>460</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -8679,7 +8672,7 @@
         <v>76</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>77</v>
@@ -8697,13 +8690,13 @@
         <v>76</v>
       </c>
       <c r="AL58" t="s" s="2">
+        <v>460</v>
+      </c>
+      <c r="AM58" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AN58" t="s" s="2">
         <v>461</v>
-      </c>
-      <c r="AM58" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN58" t="s" s="2">
-        <v>462</v>
       </c>
       <c r="AO58" t="s" s="2">
         <v>76</v>
@@ -8711,10 +8704,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8826,10 +8819,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8943,10 +8936,10 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -9062,10 +9055,10 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -9088,13 +9081,13 @@
         <v>76</v>
       </c>
       <c r="K62" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="L62" t="s" s="2">
         <v>467</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="M62" t="s" s="2">
         <v>468</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>469</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
@@ -9145,7 +9138,7 @@
         <v>76</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>86</v>
@@ -9163,7 +9156,7 @@
         <v>76</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>76</v>
@@ -9177,10 +9170,10 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9206,10 +9199,10 @@
         <v>180</v>
       </c>
       <c r="L63" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="M63" t="s" s="2">
         <v>472</v>
-      </c>
-      <c r="M63" t="s" s="2">
-        <v>473</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -9239,11 +9232,11 @@
         <v>174</v>
       </c>
       <c r="Y63" t="s" s="2">
+        <v>473</v>
+      </c>
+      <c r="Z63" t="s" s="2">
         <v>474</v>
       </c>
-      <c r="Z63" t="s" s="2">
-        <v>475</v>
-      </c>
       <c r="AA63" t="s" s="2">
         <v>76</v>
       </c>
@@ -9260,7 +9253,7 @@
         <v>76</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>77</v>
@@ -9284,18 +9277,18 @@
         <v>76</v>
       </c>
       <c r="AN63" t="s" s="2">
+        <v>475</v>
+      </c>
+      <c r="AO63" t="s" s="2">
         <v>476</v>
-      </c>
-      <c r="AO63" t="s" s="2">
-        <v>477</v>
       </c>
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9321,10 +9314,10 @@
         <v>180</v>
       </c>
       <c r="L64" t="s" s="2">
+        <v>478</v>
+      </c>
+      <c r="M64" t="s" s="2">
         <v>479</v>
-      </c>
-      <c r="M64" t="s" s="2">
-        <v>480</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
@@ -9354,11 +9347,11 @@
         <v>174</v>
       </c>
       <c r="Y64" t="s" s="2">
+        <v>480</v>
+      </c>
+      <c r="Z64" t="s" s="2">
         <v>481</v>
       </c>
-      <c r="Z64" t="s" s="2">
-        <v>482</v>
-      </c>
       <c r="AA64" t="s" s="2">
         <v>76</v>
       </c>
@@ -9375,7 +9368,7 @@
         <v>76</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>77</v>
@@ -9393,13 +9386,13 @@
         <v>76</v>
       </c>
       <c r="AL64" t="s" s="2">
+        <v>482</v>
+      </c>
+      <c r="AM64" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AN64" t="s" s="2">
         <v>483</v>
-      </c>
-      <c r="AM64" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN64" t="s" s="2">
-        <v>484</v>
       </c>
       <c r="AO64" t="s" s="2">
         <v>76</v>
@@ -9407,10 +9400,10 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9433,13 +9426,13 @@
         <v>76</v>
       </c>
       <c r="K65" t="s" s="2">
+        <v>485</v>
+      </c>
+      <c r="L65" t="s" s="2">
         <v>486</v>
       </c>
-      <c r="L65" t="s" s="2">
+      <c r="M65" t="s" s="2">
         <v>487</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>488</v>
       </c>
       <c r="N65" s="2"/>
       <c r="O65" s="2"/>
@@ -9490,7 +9483,7 @@
         <v>76</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>77</v>
@@ -9508,13 +9501,13 @@
         <v>76</v>
       </c>
       <c r="AL65" t="s" s="2">
+        <v>488</v>
+      </c>
+      <c r="AM65" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AN65" t="s" s="2">
         <v>489</v>
-      </c>
-      <c r="AM65" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AN65" t="s" s="2">
-        <v>490</v>
       </c>
       <c r="AO65" t="s" s="2">
         <v>76</v>
@@ -9522,14 +9515,14 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" t="s" s="2">
@@ -9548,16 +9541,16 @@
         <v>76</v>
       </c>
       <c r="K66" t="s" s="2">
+        <v>492</v>
+      </c>
+      <c r="L66" t="s" s="2">
         <v>493</v>
       </c>
-      <c r="L66" t="s" s="2">
+      <c r="M66" t="s" s="2">
         <v>494</v>
       </c>
-      <c r="M66" t="s" s="2">
+      <c r="N66" t="s" s="2">
         <v>495</v>
-      </c>
-      <c r="N66" t="s" s="2">
-        <v>496</v>
       </c>
       <c r="O66" s="2"/>
       <c r="P66" t="s" s="2">
@@ -9607,7 +9600,7 @@
         <v>76</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>77</v>
@@ -9625,7 +9618,7 @@
         <v>76</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="AM66" t="s" s="2">
         <v>76</v>
@@ -9639,10 +9632,10 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -9665,16 +9658,16 @@
         <v>76</v>
       </c>
       <c r="K67" t="s" s="2">
+        <v>498</v>
+      </c>
+      <c r="L67" t="s" s="2">
         <v>499</v>
       </c>
-      <c r="L67" t="s" s="2">
+      <c r="M67" t="s" s="2">
         <v>500</v>
       </c>
-      <c r="M67" t="s" s="2">
+      <c r="N67" t="s" s="2">
         <v>501</v>
-      </c>
-      <c r="N67" t="s" s="2">
-        <v>502</v>
       </c>
       <c r="O67" s="2"/>
       <c r="P67" t="s" s="2">
@@ -9724,7 +9717,7 @@
         <v>76</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>77</v>
@@ -9742,7 +9735,7 @@
         <v>76</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AM67" t="s" s="2">
         <v>76</v>

</xml_diff>